<commit_message>
ajax loding image and admin message
</commit_message>
<xml_diff>
--- a/bdApi/files/Donors.xlsx
+++ b/bdApi/files/Donors.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Dob</t>
   </si>
   <si>
-    <t>Vijayawada</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -58,6 +55,15 @@
   </si>
   <si>
     <t>Test User</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>kukatlapally</t>
   </si>
 </sst>
 </file>
@@ -389,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -400,12 +406,13 @@
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -416,44 +423,50 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>1234567890</v>
+      </c>
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="B2">
-        <v>9959167377</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>